<commit_message>
Erreur de frappe corrigée
</commit_message>
<xml_diff>
--- a/Copie de Compte Github Master 2.xlsx
+++ b/Copie de Compte Github Master 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\IRISMASTER2\DemoBidon\DemoBidon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1FA32542-0E90-4E47-B7CA-858B3746CDC6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{52CA83F7-477C-4D1D-AF6A-8A7F2ACAC02E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5664" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -150,7 +150,7 @@
     <t>Nivedita</t>
   </si>
   <si>
-    <t>https://github.com/kyou705</t>
+    <t>https://github.com/kyou705?tab=repositories</t>
   </si>
 </sst>
 </file>

</xml_diff>